<commit_message>
Fix bug when login and Review Code #1
</commit_message>
<xml_diff>
--- a/Library-ProjectI/template/library.xlsx
+++ b/Library-ProjectI/template/library.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="115">
   <si>
     <t>Mã sách</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Thể loại</t>
   </si>
   <si>
-    <t>LT09</t>
-  </si>
-  <si>
     <t>Vue.JS</t>
   </si>
   <si>
@@ -51,12 +48,6 @@
     <t>Bách Khoa</t>
   </si>
   <si>
-    <t>Tự Nhiên</t>
-  </si>
-  <si>
-    <t>LT10</t>
-  </si>
-  <si>
     <t>HTML-CSS</t>
   </si>
   <si>
@@ -108,12 +99,6 @@
     <t>Hà Nội</t>
   </si>
   <si>
-    <t>0123456456789</t>
-  </si>
-  <si>
-    <t>012345879452</t>
-  </si>
-  <si>
     <t>DG08</t>
   </si>
   <si>
@@ -147,13 +132,235 @@
     <t>01234897611</t>
   </si>
   <si>
-    <t>0123456874</t>
-  </si>
-  <si>
-    <t>NV09</t>
-  </si>
-  <si>
-    <t>NV08</t>
+    <t>LT01</t>
+  </si>
+  <si>
+    <t>LT02</t>
+  </si>
+  <si>
+    <t>Lập trình</t>
+  </si>
+  <si>
+    <t>LT03</t>
+  </si>
+  <si>
+    <t>Java Script</t>
+  </si>
+  <si>
+    <t>Đinh Thanh Nam</t>
+  </si>
+  <si>
+    <t>LT04</t>
+  </si>
+  <si>
+    <t>OOP với Java</t>
+  </si>
+  <si>
+    <t>LT05</t>
+  </si>
+  <si>
+    <t>Front-End với HTML5 và CSS3</t>
+  </si>
+  <si>
+    <t>LT06</t>
+  </si>
+  <si>
+    <t>NodeJS</t>
+  </si>
+  <si>
+    <t>D. Luiz</t>
+  </si>
+  <si>
+    <t>Thanh Niên</t>
+  </si>
+  <si>
+    <t>VH01</t>
+  </si>
+  <si>
+    <t>Củ cải đường</t>
+  </si>
+  <si>
+    <t>Nguyễn Linh Thu</t>
+  </si>
+  <si>
+    <t>Văn học</t>
+  </si>
+  <si>
+    <t>VH02</t>
+  </si>
+  <si>
+    <t>Cơn mưa ngang qua</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Tùng</t>
+  </si>
+  <si>
+    <t>Kim Đồng</t>
+  </si>
+  <si>
+    <t>VH03</t>
+  </si>
+  <si>
+    <t>Ngồi cười trên cây</t>
+  </si>
+  <si>
+    <t>Nguyễn Thu Minh</t>
+  </si>
+  <si>
+    <t>VH04</t>
+  </si>
+  <si>
+    <t>Định mệnh</t>
+  </si>
+  <si>
+    <t>Trần Thanh Nhàn</t>
+  </si>
+  <si>
+    <t>XH01</t>
+  </si>
+  <si>
+    <t>Bệnh béo phì</t>
+  </si>
+  <si>
+    <t>Trần Thanh Tâm</t>
+  </si>
+  <si>
+    <t>Xã hội</t>
+  </si>
+  <si>
+    <t>XH02</t>
+  </si>
+  <si>
+    <t>Bệnh tim mạch</t>
+  </si>
+  <si>
+    <t>Trần Trung Kiên</t>
+  </si>
+  <si>
+    <t>Trẻ</t>
+  </si>
+  <si>
+    <t>XH03</t>
+  </si>
+  <si>
+    <t>Tâm lí học tội phạm</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>Tuyển tập Cổ tích Việt Nam</t>
+  </si>
+  <si>
+    <t>Truyện</t>
+  </si>
+  <si>
+    <t>TC02</t>
+  </si>
+  <si>
+    <t>Truyện cười Dân gian</t>
+  </si>
+  <si>
+    <t>DG01</t>
+  </si>
+  <si>
+    <t>01234564567</t>
+  </si>
+  <si>
+    <t>01234587945</t>
+  </si>
+  <si>
+    <t>DG02</t>
+  </si>
+  <si>
+    <t>DG03</t>
+  </si>
+  <si>
+    <t>Vũ Hoàng Giang</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>DG04</t>
+  </si>
+  <si>
+    <t>Kim Suyn Jun</t>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>01667689125</t>
+  </si>
+  <si>
+    <t>01235684892</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Thìn</t>
+  </si>
+  <si>
+    <t>Thái Bình</t>
+  </si>
+  <si>
+    <t>01895632478</t>
+  </si>
+  <si>
+    <t>DG06</t>
+  </si>
+  <si>
+    <t>Nguyễn Thu Mai</t>
+  </si>
+  <si>
+    <t>01289654233</t>
+  </si>
+  <si>
+    <t>DG07</t>
+  </si>
+  <si>
+    <t>Vũ Thị Nhung</t>
+  </si>
+  <si>
+    <t>01598743621</t>
+  </si>
+  <si>
+    <t>Phan Thanh Nam</t>
+  </si>
+  <si>
+    <t>Hải Phòng</t>
+  </si>
+  <si>
+    <t>01259874632</t>
+  </si>
+  <si>
+    <t>NV01</t>
+  </si>
+  <si>
+    <t>NV02</t>
+  </si>
+  <si>
+    <t>01234568745</t>
+  </si>
+  <si>
+    <t>NV03</t>
+  </si>
+  <si>
+    <t>Trịnh Thu Trang</t>
+  </si>
+  <si>
+    <t>Thanh Hóa</t>
+  </si>
+  <si>
+    <t>01235488945</t>
+  </si>
+  <si>
+    <t>NV04</t>
+  </si>
+  <si>
+    <t>Văn Mai Hương</t>
+  </si>
+  <si>
+    <t>01687945615</t>
   </si>
 </sst>
 </file>
@@ -538,26 +745,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -591,19 +798,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F4">
         <v>2016</v>
@@ -614,25 +821,324 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="F5">
         <v>2014</v>
       </c>
       <c r="G5">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>2014</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>2015</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>2015</v>
+      </c>
+      <c r="G8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>2017</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10">
+        <v>2014</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11">
+        <v>2012</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12">
+        <v>2016</v>
+      </c>
+      <c r="G12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13">
+        <v>2013</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14">
+        <v>2011</v>
+      </c>
+      <c r="G14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15">
+        <v>2013</v>
+      </c>
+      <c r="G15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16">
+        <v>2011</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17">
+        <v>2011</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18">
+        <v>2013</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -645,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +1169,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -674,71 +1180,209 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>1976</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>1998</v>
       </c>
       <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6">
+        <v>1997</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7">
+        <v>1990</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8">
+        <v>1997</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9">
+        <v>1998</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>1999</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>31</v>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11">
+        <v>1997</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -751,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +1412,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -779,71 +1423,117 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C4">
         <v>1995</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>1984</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6">
+        <v>1995</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7">
+        <v>1994</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>